<commit_message>
Initial work to implement Monte Carlo analysis - generate iterations for one table.
</commit_message>
<xml_diff>
--- a/Data/CostData/BaselineDatabase.xlsx
+++ b/Data/CostData/BaselineDatabase.xlsx
@@ -20,17 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="125">
   <si>
     <t>ScenarioID</t>
   </si>
   <si>
+    <t>Scenario_Name</t>
+  </si>
+  <si>
     <t>Scenario_Tag</t>
   </si>
   <si>
-    <t>Scenario_Name</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -43,6 +43,18 @@
     <t>4</t>
   </si>
   <si>
+    <t>MAV 14.4GW in 2024</t>
+  </si>
+  <si>
+    <t>SAT 10.5GW in 2024</t>
+  </si>
+  <si>
+    <t>MAV 14.4GW over 5 years</t>
+  </si>
+  <si>
+    <t>SAT 10.5GW in over 5 years</t>
+  </si>
+  <si>
     <t>M1</t>
   </si>
   <si>
@@ -55,30 +67,45 @@
     <t>S5</t>
   </si>
   <si>
-    <t>MAV 14.4GW in 2024</t>
-  </si>
-  <si>
-    <t>SAT 10.5GW in 2024</t>
-  </si>
-  <si>
-    <t>MAV 14.4GW over 5 years</t>
-  </si>
-  <si>
-    <t>SAT 10.5GW in over 5 years</t>
+    <t>System_Name</t>
+  </si>
+  <si>
+    <t>System_Tag</t>
   </si>
   <si>
     <t>System_Description</t>
   </si>
   <si>
-    <t>System_Tag</t>
-  </si>
-  <si>
-    <t>System_Name</t>
-  </si>
-  <si>
     <t>SystemID</t>
   </si>
   <si>
+    <t>20MW MAV Block (1 size)</t>
+  </si>
+  <si>
+    <t>20MW SAT block</t>
+  </si>
+  <si>
+    <t>20MW MAV Block (1.2 size)</t>
+  </si>
+  <si>
+    <t>Work Camp</t>
+  </si>
+  <si>
+    <t>Decomission workcamp</t>
+  </si>
+  <si>
+    <t>SAT1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
     <t>20MW DC</t>
   </si>
   <si>
@@ -88,33 +115,6 @@
     <t xml:space="preserve">for 100 people. </t>
   </si>
   <si>
-    <t>SAT1</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>W1</t>
-  </si>
-  <si>
-    <t>W2</t>
-  </si>
-  <si>
-    <t>20MW MAV Block (1 size)</t>
-  </si>
-  <si>
-    <t>20MW SAT block</t>
-  </si>
-  <si>
-    <t>20MW MAV Block (1.2 size)</t>
-  </si>
-  <si>
-    <t>Work Camp</t>
-  </si>
-  <si>
-    <t>Decomission workcamp</t>
-  </si>
-  <si>
     <t>ScenarioSystemID</t>
   </si>
   <si>
@@ -124,58 +124,37 @@
     <t>InstallNumber</t>
   </si>
   <si>
+    <t>ComponentID</t>
+  </si>
+  <si>
+    <t>AnnualMultiplier_H</t>
+  </si>
+  <si>
     <t>BaselineYear</t>
   </si>
   <si>
+    <t>CurrencyID</t>
+  </si>
+  <si>
+    <t>AnnualMultiplier</t>
+  </si>
+  <si>
+    <t>FutureCostMethod</t>
+  </si>
+  <si>
+    <t>Component_Comment</t>
+  </si>
+  <si>
+    <t>AnnualMultiplier_L</t>
+  </si>
+  <si>
+    <t>Component_Name</t>
+  </si>
+  <si>
+    <t>BaselineCost</t>
+  </si>
+  <si>
     <t>Component_Unit</t>
-  </si>
-  <si>
-    <t>AnnualMultiplier</t>
-  </si>
-  <si>
-    <t>FutureCostMethod</t>
-  </si>
-  <si>
-    <t>ComponentID</t>
-  </si>
-  <si>
-    <t>CurrencyID</t>
-  </si>
-  <si>
-    <t>BaselineCost</t>
-  </si>
-  <si>
-    <t>Component_Comment</t>
-  </si>
-  <si>
-    <t>Component_Name</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>MAV</t>
-  </si>
-  <si>
-    <t>hour</t>
-  </si>
-  <si>
-    <t>hour of use</t>
-  </si>
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>MW.year</t>
-  </si>
-  <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>Per 100 camp</t>
-  </si>
-  <si>
-    <t>per 100 camp</t>
   </si>
   <si>
     <t>Baseline module</t>
@@ -292,22 +271,64 @@
     <t>Workcamp decommission</t>
   </si>
   <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>MAV</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>hour of use</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>MW.year</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>Per 100 camp</t>
+  </si>
+  <si>
+    <t>per 100 camp</t>
+  </si>
+  <si>
+    <t>Config_Name (from Config_link)</t>
+  </si>
+  <si>
+    <t>CostCategoryID</t>
+  </si>
+  <si>
     <t>Timing</t>
   </si>
   <si>
+    <t>TimingYear</t>
+  </si>
+  <si>
     <t>Usage</t>
   </si>
   <si>
-    <t>CostCategoryID</t>
-  </si>
-  <si>
-    <t>Config_Name (from Config_link)</t>
-  </si>
-  <si>
     <t>SystemComponentID</t>
   </si>
   <si>
-    <t>TimingYear</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
   <si>
     <t>Installation</t>
@@ -316,21 +337,6 @@
     <t>PerOperationYear</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>To_AUD</t>
   </si>
   <si>
@@ -343,18 +349,39 @@
     <t>USD</t>
   </si>
   <si>
+    <t>CostCategory_ShortName</t>
+  </si>
+  <si>
     <t>CostCategory_Name</t>
   </si>
   <si>
-    <t>CostCategory_ShortName</t>
-  </si>
-  <si>
     <t>Modules</t>
   </si>
   <si>
     <t>BOS Hardware</t>
   </si>
   <si>
+    <t>MAV Lic</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>NOT USED</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Allowances</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>MAV Licencre</t>
   </si>
   <si>
@@ -364,12 +391,6 @@
     <t>System Deployment - Hardware</t>
   </si>
   <si>
-    <t>NOT USED</t>
-  </si>
-  <si>
-    <t>Maintenance</t>
-  </si>
-  <si>
     <t>Logistics Site</t>
   </si>
   <si>
@@ -377,21 +398,6 @@
   </si>
   <si>
     <t>EPC Overhead</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>MAV Lic</t>
-  </si>
-  <si>
-    <t>Logistics</t>
-  </si>
-  <si>
-    <t>Site</t>
-  </si>
-  <si>
-    <t>Allowances</t>
   </si>
 </sst>
 </file>
@@ -857,10 +863,10 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -871,13 +877,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>8</v>
@@ -888,13 +894,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>9</v>
@@ -905,13 +911,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>11</v>
@@ -921,14 +927,14 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
-        <v>0</v>
+      <c r="B6" t="s">
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6">
         <v>12</v>
@@ -949,479 +955,479 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>2024</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>720</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
+      <c r="E3">
         <v>2025</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
         <v>2026</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
+      <c r="E5">
         <v>2027</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6">
+      <c r="E6">
         <v>2024</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>525</v>
-      </c>
-      <c r="F6">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7">
+      <c r="E7">
         <v>2025</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
       <c r="F7">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8">
+      <c r="E8">
         <v>2026</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
       <c r="F8">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
       <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
         <v>2027</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
       <c r="F9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10">
+      <c r="E10">
         <v>2024</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>144</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11">
+      <c r="E11">
         <v>2025</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>144</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
+      <c r="E12">
         <v>2026</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>144</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
+      <c r="E13">
         <v>2027</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>144</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14">
+      <c r="E14">
         <v>2028</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
+      <c r="E15">
         <v>2028</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>144</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
         <v>15</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16">
+      <c r="E16">
         <v>2024</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>105</v>
-      </c>
-      <c r="F16">
-        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
         <v>16</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17">
+      <c r="E17">
         <v>2025</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>105</v>
-      </c>
-      <c r="F17">
-        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18">
+      <c r="E18">
         <v>2026</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>105</v>
-      </c>
-      <c r="F18">
-        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+      <c r="D19">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19">
+      <c r="E19">
         <v>2027</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>105</v>
-      </c>
-      <c r="F19">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20">
+      <c r="E20">
         <v>2028</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>105</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" t="s">
         <v>5</v>
       </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
       <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21">
         <v>2024</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>2</v>
-      </c>
-      <c r="F21">
-        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
         <v>21</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22">
+      <c r="E22">
         <v>2024</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>2</v>
-      </c>
-      <c r="F22">
-        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+      <c r="D23">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23">
+      <c r="E23">
         <v>2028</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>5</v>
-      </c>
-      <c r="F23">
-        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
         <v>23</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24">
+      <c r="E24">
         <v>2026</v>
       </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
       <c r="F24">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1431,13 +1437,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1465,773 +1471,923 @@
       <c r="J1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.9</v>
+      </c>
+      <c r="D2">
         <v>2024</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2">
         <v>0.83</v>
       </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2">
+        <v>38</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="J2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2">
         <v>0.18</v>
       </c>
-      <c r="I2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="L2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1.01</v>
+      </c>
+      <c r="D3">
         <v>2020</v>
       </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3">
+        <v>0.99</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3">
         <v>4551</v>
       </c>
-      <c r="I3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1.01</v>
+      </c>
+      <c r="D4">
         <v>2020</v>
       </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0.99</v>
+      </c>
+      <c r="J4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4">
         <v>150</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1.01</v>
+      </c>
+      <c r="D5">
         <v>2020</v>
       </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0.99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5">
         <v>200</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1.01</v>
+      </c>
+      <c r="D6">
         <v>2020</v>
       </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6">
+        <v>0.99</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="L6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>1.01</v>
+      </c>
+      <c r="D7">
         <v>2020</v>
       </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.99</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7">
         <v>1.5</v>
       </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="L7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1.01</v>
+      </c>
+      <c r="D8">
         <v>2024</v>
       </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8">
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8">
         <v>0.83</v>
       </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
       <c r="G8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8">
+        <v>0.99</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
+      </c>
+      <c r="K8">
         <v>99</v>
       </c>
-      <c r="I8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="L8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>1.01</v>
+      </c>
+      <c r="D9">
         <v>2024</v>
       </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9">
+        <v>38</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9">
+        <v>0.99</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9">
         <v>4.3</v>
       </c>
-      <c r="I9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>1.01</v>
+      </c>
+      <c r="D10">
         <v>2024</v>
       </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F10">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>0.99</v>
+      </c>
+      <c r="J10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10">
         <v>138</v>
       </c>
-      <c r="I10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="L10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>1.01</v>
+      </c>
+      <c r="D11">
         <v>2024</v>
       </c>
-      <c r="C11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11">
+        <v>38</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11">
+        <v>0.99</v>
+      </c>
+      <c r="J11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11">
         <v>68.8</v>
       </c>
-      <c r="I11" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="L11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <v>1.01</v>
+      </c>
+      <c r="D12">
         <v>2024</v>
       </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.99</v>
+      </c>
+      <c r="J12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12">
         <v>7000</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="L12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <v>1.01</v>
+      </c>
+      <c r="D13">
         <v>2024</v>
       </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0.99</v>
+      </c>
+      <c r="J13" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13">
         <v>5000</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="L13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>1.01</v>
+      </c>
+      <c r="D14">
         <v>2024</v>
       </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F14">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0.99</v>
+      </c>
+      <c r="J14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K14">
         <v>25000</v>
       </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-      <c r="J14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="L14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>1.01</v>
+      </c>
+      <c r="D15">
         <v>2024</v>
       </c>
-      <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0.99</v>
+      </c>
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15">
         <v>30000</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="L15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>1.01</v>
+      </c>
+      <c r="D16">
         <v>2024</v>
       </c>
-      <c r="C16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0.99</v>
+      </c>
+      <c r="J16" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16">
         <v>80300</v>
       </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="L16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>1.01</v>
+      </c>
+      <c r="D17">
         <v>2024</v>
       </c>
-      <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17">
+        <v>38</v>
+      </c>
+      <c r="H17" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17">
+        <v>0.99</v>
+      </c>
+      <c r="J17" t="s">
+        <v>73</v>
+      </c>
+      <c r="K17">
         <v>20000</v>
       </c>
-      <c r="I17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="L17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>1.01</v>
+      </c>
+      <c r="D18">
         <v>2020</v>
       </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F18">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0.99</v>
+      </c>
+      <c r="J18" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18">
         <v>100</v>
       </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="L18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <v>1.01</v>
+      </c>
+      <c r="D19">
         <v>2024</v>
       </c>
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19">
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19">
+        <v>0.99</v>
+      </c>
+      <c r="J19" t="s">
+        <v>75</v>
+      </c>
+      <c r="K19">
         <v>114</v>
       </c>
-      <c r="I19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="L19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>1.01</v>
+      </c>
+      <c r="D20">
         <v>2024</v>
       </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
       <c r="E20" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20">
+        <v>38</v>
+      </c>
+      <c r="H20" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20">
+        <v>0.99</v>
+      </c>
+      <c r="J20" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20">
         <v>61.5</v>
       </c>
-      <c r="I20" t="s">
-        <v>61</v>
-      </c>
-      <c r="J20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="L20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21">
+        <v>27</v>
+      </c>
+      <c r="C21">
+        <v>1.01</v>
+      </c>
+      <c r="D21">
         <v>2024</v>
       </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F21">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21">
+        <v>38</v>
+      </c>
+      <c r="H21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I21">
+        <v>0.99</v>
+      </c>
+      <c r="J21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21">
         <v>131</v>
       </c>
-      <c r="I21" t="s">
-        <v>62</v>
-      </c>
-      <c r="J21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="L21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>1.01</v>
+      </c>
+      <c r="D22">
         <v>2024</v>
       </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F22">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H22">
+        <v>38</v>
+      </c>
+      <c r="H22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22">
+        <v>0.99</v>
+      </c>
+      <c r="J22" t="s">
+        <v>78</v>
+      </c>
+      <c r="K22">
         <v>262</v>
       </c>
-      <c r="I22" t="s">
-        <v>63</v>
-      </c>
-      <c r="J22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="L22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>0.9</v>
+      </c>
+      <c r="D23">
         <v>2024</v>
       </c>
-      <c r="C23" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23">
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23">
         <v>0.83</v>
       </c>
-      <c r="E23" t="s">
-        <v>36</v>
-      </c>
-      <c r="F23">
-        <v>29</v>
-      </c>
       <c r="G23" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23">
+        <v>38</v>
+      </c>
+      <c r="H23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="J23" t="s">
+        <v>79</v>
+      </c>
+      <c r="K23">
         <v>7.43</v>
       </c>
-      <c r="I23" t="s">
-        <v>64</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="L23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24">
+        <v>1.01</v>
+      </c>
+      <c r="D24">
         <v>2024</v>
       </c>
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0.99</v>
+      </c>
+      <c r="J24" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24">
         <v>10000000</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="L24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
+        <v>31</v>
+      </c>
+      <c r="C25">
+        <v>1.01</v>
+      </c>
+      <c r="D25">
         <v>2024</v>
       </c>
-      <c r="C25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0.99</v>
+      </c>
+      <c r="J25" t="s">
+        <v>81</v>
+      </c>
+      <c r="K25">
         <v>1000000</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25" t="s">
-        <v>88</v>
+      <c r="L25" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2249,219 +2405,219 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3">
-        <v>303</v>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3">
+        <v>303</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C4">
-        <v>1769</v>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>1769</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5">
-        <v>269</v>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5">
+        <v>269</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>4</v>
-      </c>
-      <c r="H5">
-        <v>4</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6">
-        <v>531</v>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6">
+        <v>531</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>14</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7">
-        <v>531</v>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
       </c>
       <c r="D7" t="s">
         <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
+        <v>531</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
         <v>15</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8">
-        <v>20</v>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -2470,706 +2626,706 @@
         <v>20</v>
       </c>
       <c r="H8">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>36364</v>
       </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>28</v>
-      </c>
-      <c r="H9">
-        <v>7</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>36364</v>
       </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10">
+      <c r="H10">
         <v>8</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>29</v>
-      </c>
-      <c r="H10">
-        <v>7</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11">
-        <v>2037</v>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>97</v>
       </c>
       <c r="E11" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2037</v>
+      </c>
+      <c r="H11">
         <v>8</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>30</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12">
-        <v>386</v>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
       </c>
       <c r="D12" t="s">
         <v>97</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>386</v>
+      </c>
+      <c r="H12">
         <v>8</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>31</v>
-      </c>
-      <c r="H12">
-        <v>4</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13">
-        <v>116</v>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>97</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>116</v>
+      </c>
+      <c r="H13">
         <v>8</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>32</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>95</v>
-      </c>
-      <c r="C14">
-        <v>116</v>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
       </c>
       <c r="D14" t="s">
         <v>97</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>116</v>
+      </c>
+      <c r="H14">
         <v>8</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>33</v>
-      </c>
-      <c r="H14">
-        <v>6</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15">
-        <v>20</v>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
       </c>
       <c r="D15" t="s">
         <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <v>34</v>
-      </c>
-      <c r="H15">
-        <v>16</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16">
-        <v>20</v>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
       </c>
       <c r="D16" t="s">
         <v>98</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
         <v>35</v>
-      </c>
-      <c r="H16">
-        <v>17</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17">
-        <v>20</v>
+      <c r="B17">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>36</v>
-      </c>
-      <c r="H17">
-        <v>18</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C18">
-        <v>20</v>
+      <c r="B18">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
       </c>
       <c r="D18" t="s">
         <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>37</v>
-      </c>
-      <c r="H18">
-        <v>19</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C19">
-        <v>20</v>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
       </c>
       <c r="D19" t="s">
         <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19">
+        <v>20</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
         <v>38</v>
-      </c>
-      <c r="H19">
-        <v>20</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20">
-        <v>20</v>
+      <c r="B20">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
       </c>
       <c r="D20" t="s">
         <v>101</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>39</v>
-      </c>
-      <c r="H20">
-        <v>21</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C21">
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" t="s">
         <v>100</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="H21">
         <v>8</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>40</v>
-      </c>
-      <c r="H21">
-        <v>20</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22">
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
         <v>20</v>
       </c>
       <c r="D22" t="s">
         <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>20</v>
+      </c>
+      <c r="H22">
         <v>8</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>41</v>
-      </c>
-      <c r="H22">
-        <v>21</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23">
+      <c r="B23">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23" t="s">
         <v>99</v>
       </c>
       <c r="E23" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>20</v>
+      </c>
+      <c r="H23">
         <v>8</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>42</v>
-      </c>
-      <c r="H23">
-        <v>23</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24">
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>20</v>
+      </c>
+      <c r="H24">
         <v>8</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <v>43</v>
-      </c>
-      <c r="H24">
-        <v>22</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25">
-        <v>7919</v>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
       </c>
       <c r="D25" t="s">
         <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>7919</v>
+      </c>
+      <c r="H25">
         <v>8</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>44</v>
-      </c>
-      <c r="H25">
-        <v>24</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26">
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
         <v>20</v>
       </c>
       <c r="D26" t="s">
         <v>97</v>
       </c>
       <c r="E26" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>20</v>
+      </c>
+      <c r="H26">
         <v>8</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>45</v>
-      </c>
-      <c r="H26">
-        <v>25</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27">
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
         <v>20</v>
       </c>
       <c r="D27" t="s">
         <v>98</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>20</v>
+      </c>
+      <c r="H27">
         <v>8</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>49</v>
-      </c>
-      <c r="H27">
-        <v>26</v>
-      </c>
-      <c r="I27">
-        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28">
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
         <v>20</v>
       </c>
       <c r="D28" t="s">
         <v>98</v>
       </c>
       <c r="E28" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="H28">
         <v>8</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>50</v>
-      </c>
-      <c r="H28">
-        <v>27</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29">
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
         <v>20</v>
       </c>
       <c r="D29" t="s">
         <v>98</v>
       </c>
       <c r="E29" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>20</v>
+      </c>
+      <c r="H29">
         <v>8</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>51</v>
-      </c>
-      <c r="H29">
-        <v>28</v>
-      </c>
-      <c r="I29">
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30">
-        <v>36364</v>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30">
+        <v>36364</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
         <v>53</v>
-      </c>
-      <c r="H30">
-        <v>29</v>
-      </c>
-      <c r="I30">
-        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>22</v>
       </c>
       <c r="D31" t="s">
         <v>99</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
         <v>11</v>
       </c>
-      <c r="G31">
+      <c r="I31">
         <v>54</v>
-      </c>
-      <c r="H31">
-        <v>30</v>
-      </c>
-      <c r="I31">
-        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
       </c>
       <c r="D32" t="s">
         <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
         <v>12</v>
       </c>
-      <c r="G32">
+      <c r="I32">
         <v>55</v>
-      </c>
-      <c r="H32">
-        <v>31</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3187,41 +3343,41 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>37</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>1.35</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3239,13 +3395,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3253,13 +3409,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3267,13 +3423,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3281,7 +3437,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -3295,7 +3451,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -3309,7 +3465,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
         <v>97</v>
@@ -3323,13 +3479,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
         <v>118</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3337,13 +3493,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
         <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3351,13 +3507,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C9" t="s">
         <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3365,13 +3521,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3385,7 +3541,7 @@
         <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>